<commit_message>
C program test files
</commit_message>
<xml_diff>
--- a/sw/c_program/Used Instructions.xlsx
+++ b/sw/c_program/Used Instructions.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Courses\S2\ELEC6231 VLSI Design Project\ARC\sw\c_program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Courses\S2\ELEC6231 VLSI Design Project\ARC\sw\c_program\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="test_c_assembly" localSheetId="0">Sheet2!$A$1:$A$44</definedName>
+    <definedName name="test_c_assembly_1" localSheetId="0">Sheet2!$A$1:$A$145</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,8 +30,11 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="test_c_assembly" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="Y:\Courses\S2\ELEC6231 VLSI Design Project\ARC\sw\c_program\test_c_assembly.txt">
-      <textFields>
+    <textPr codePage="850" sourceFile="H:\Courses\S2\ELEC6231 VLSI Design Project\ARC\sw\c_program\test_c_assembly.txt">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
       </textFields>
     </textPr>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>addiu</t>
   </si>
@@ -63,16 +66,43 @@
     <t>subu</t>
   </si>
   <si>
-    <t>lui</t>
-  </si>
-  <si>
-    <t>sb</t>
-  </si>
-  <si>
-    <t>lbu</t>
-  </si>
-  <si>
     <t>jr</t>
+  </si>
+  <si>
+    <t>addu</t>
+  </si>
+  <si>
+    <t>mult</t>
+  </si>
+  <si>
+    <t>mflo</t>
+  </si>
+  <si>
+    <t>sll</t>
+  </si>
+  <si>
+    <t>bnez</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t>srl</t>
+  </si>
+  <si>
+    <t>sra</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>bgtz</t>
+  </si>
+  <si>
+    <t>slt</t>
   </si>
 </sst>
 </file>
@@ -128,7 +158,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_c_assembly" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_c_assembly_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,15 +424,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -437,36 +468,83 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>